<commit_message>
Updated sample manual data
</commit_message>
<xml_diff>
--- a/public/data/manual/2020/FEB/10071309.xlsx
+++ b/public/data/manual/2020/FEB/10071309.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dftools\public\data\manual\2020\FEB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin.dizon\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4864939-C015-4AD8-9792-C132EAD2015C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02D8856-B0D6-4DD2-865A-7D637F31C0C3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="-930" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WEIGHT" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Employee ID</t>
   </si>
@@ -59,13 +59,19 @@
   </si>
   <si>
     <t>DESGN</t>
+  </si>
+  <si>
+    <t>Productivity Score</t>
+  </si>
+  <si>
+    <t>Product Knowledge Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,13 +90,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -109,9 +129,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{A5FAD43E-F267-4A99-A648-9188C3FC62BC}"/>
@@ -399,7 +422,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,8 +495,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB74E00-A2C4-46DA-A1B5-583D892845CE}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631123C5-DB1A-4494-8151-0AB55CDF9F1E}">
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -482,66 +505,64 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>10072444</v>
       </c>
-      <c r="B2" s="1">
-        <v>75</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2">
+        <v>74</v>
+      </c>
+      <c r="C2">
         <v>98</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
+        <v>90</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
         <v>80</v>
       </c>
-      <c r="E2" s="1">
+      <c r="G2">
         <v>100</v>
       </c>
-      <c r="F2" s="1">
-        <v>90</v>
-      </c>
-      <c r="G2" s="1">
-        <v>100</v>
-      </c>
-      <c r="H2" s="1">
-        <f>(B2 * WEIGHT!$B$2) + (C2 * WEIGHT!$B$3) + (D2 * WEIGHT!$B$4) + (E2 * WEIGHT!$B$5) + (F2 * WEIGHT!$B$6) + (G2 * WEIGHT!$B$7)</f>
-        <v>86.55</v>
+      <c r="H2">
+        <f>(B2 * WEIGHT!$B$2)+(C2 * WEIGHT!$B$3)+(D2 * WEIGHT!$B$4)+(E2 * WEIGHT!$B$5)+(F2 * WEIGHT!$B$6)+(G2 * WEIGHT!$B$7)</f>
+        <v>86.8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -549,7 +570,7 @@
         <v>10072438</v>
       </c>
       <c r="B3">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3">
         <v>99</v>
@@ -567,8 +588,56 @@
         <v>100</v>
       </c>
       <c r="H3" s="1">
-        <f>(B3 * WEIGHT!$B$2) + (C3 * WEIGHT!$B$3) + (D3 * WEIGHT!$B$4) + (E3 * WEIGHT!$B$5) + (F3 * WEIGHT!$B$6) + (G3 * WEIGHT!$B$7)</f>
-        <v>92.9</v>
+        <f>(B3 * WEIGHT!$B$2)+(C3 * WEIGHT!$B$3)+(D3 * WEIGHT!$B$4)+(E3 * WEIGHT!$B$5)+(F3 * WEIGHT!$B$6)+(G3 * WEIGHT!$B$7)</f>
+        <v>92.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="1">
+        <f>(B4 * WEIGHT!$B$2)+(C4 * WEIGHT!$B$3)+(D4 * WEIGHT!$B$4)+(E4 * WEIGHT!$B$5)+(F4 * WEIGHT!$B$6)+(G4 * WEIGHT!$B$7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1">
+        <f>(B5 * WEIGHT!$B$2)+(C5 * WEIGHT!$B$3)+(D5 * WEIGHT!$B$4)+(E5 * WEIGHT!$B$5)+(F5 * WEIGHT!$B$6)+(G5 * WEIGHT!$B$7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="1">
+        <f>(B6 * WEIGHT!$B$2)+(C6 * WEIGHT!$B$3)+(D6 * WEIGHT!$B$4)+(E6 * WEIGHT!$B$5)+(F6 * WEIGHT!$B$6)+(G6 * WEIGHT!$B$7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="1">
+        <f>(B7 * WEIGHT!$B$2)+(C7 * WEIGHT!$B$3)+(D7 * WEIGHT!$B$4)+(E7 * WEIGHT!$B$5)+(F7 * WEIGHT!$B$6)+(G7 * WEIGHT!$B$7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="1">
+        <f>(B8 * WEIGHT!$B$2)+(C8 * WEIGHT!$B$3)+(D8 * WEIGHT!$B$4)+(E8 * WEIGHT!$B$5)+(F8 * WEIGHT!$B$6)+(G8 * WEIGHT!$B$7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="1">
+        <f>(B9 * WEIGHT!$B$2)+(C9 * WEIGHT!$B$3)+(D9 * WEIGHT!$B$4)+(E9 * WEIGHT!$B$5)+(F9 * WEIGHT!$B$6)+(G9 * WEIGHT!$B$7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="1">
+        <f>(B10 * WEIGHT!$B$2)+(C10 * WEIGHT!$B$3)+(D10 * WEIGHT!$B$4)+(E10 * WEIGHT!$B$5)+(F10 * WEIGHT!$B$6)+(G10 * WEIGHT!$B$7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="1">
+        <f>(B11 * WEIGHT!$B$2)+(C11 * WEIGHT!$B$3)+(D11 * WEIGHT!$B$4)+(E11 * WEIGHT!$B$5)+(F11 * WEIGHT!$B$6)+(G11 * WEIGHT!$B$7)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>